<commit_message>
add foreign key for NhapVatTu
</commit_message>
<xml_diff>
--- a/QLVatTu_KetQua.xlsx
+++ b/QLVatTu_KetQua.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="105">
   <si>
     <t>STT</t>
   </si>
@@ -732,6 +732,9 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -761,9 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1784,13 +1784,13 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="21" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="36">
         <v>3</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1799,9 +1799,9 @@
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2271,8 +2271,8 @@
   <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -2349,36 +2349,39 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="36">
         <v>3</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>83</v>
       </c>
       <c r="E7" s="7"/>
+      <c r="G7" s="34" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="35" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="3" t="s">
         <v>82</v>
       </c>
@@ -2401,6 +2404,9 @@
         <v>18</v>
       </c>
       <c r="E10" s="7"/>
+      <c r="G10" s="35" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -2459,11 +2465,11 @@
       <c r="C14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="43" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="38" t="s">
         <v>95</v>
       </c>
       <c r="G14" s="33" t="s">
@@ -2480,9 +2486,9 @@
       <c r="C15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="43"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="37"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:9" ht="21.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -2494,9 +2500,9 @@
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="37"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:10" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -2508,9 +2514,9 @@
       <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="37"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:10" ht="162.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
@@ -2576,7 +2582,7 @@
       <c r="A22" s="21">
         <v>1</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="39" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="29" t="s">
@@ -2598,7 +2604,7 @@
       <c r="A23" s="21">
         <v>2</v>
       </c>
-      <c r="B23" s="39"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="8" t="s">
         <v>15</v>
       </c>
@@ -2614,7 +2620,7 @@
       <c r="A24" s="21">
         <v>3</v>
       </c>
-      <c r="B24" s="39"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="8" t="s">
         <v>54</v>
       </c>
@@ -2627,7 +2633,7 @@
       <c r="A25" s="21">
         <v>4</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="8" t="s">
         <v>54</v>
       </c>
@@ -2640,7 +2646,7 @@
       <c r="A26" s="21">
         <v>5</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="39" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -2658,7 +2664,7 @@
       <c r="A27" s="21">
         <v>6</v>
       </c>
-      <c r="B27" s="39"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="8" t="s">
         <v>60</v>
       </c>
@@ -2671,7 +2677,7 @@
       <c r="A28" s="21">
         <v>7</v>
       </c>
-      <c r="B28" s="39"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="8" t="s">
         <v>60</v>
       </c>
@@ -2684,7 +2690,7 @@
       <c r="A29" s="21">
         <v>8</v>
       </c>
-      <c r="B29" s="39"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="8" t="s">
         <v>60</v>
       </c>
@@ -2703,7 +2709,7 @@
       <c r="A30" s="21">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
@@ -2730,7 +2736,7 @@
       <c r="A32" s="8">
         <v>1</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="39" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -2745,7 +2751,7 @@
       <c r="A33" s="8">
         <v>2</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="7" t="s">
         <v>54</v>
       </c>
@@ -2758,7 +2764,7 @@
       <c r="A34" s="8">
         <v>3</v>
       </c>
-      <c r="B34" s="40"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="7" t="s">
         <v>15</v>
       </c>
@@ -2774,7 +2780,7 @@
       <c r="A35" s="8">
         <v>4</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="39" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -2795,7 +2801,7 @@
       <c r="A36" s="8">
         <v>5</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="7" t="s">
         <v>60</v>
       </c>
@@ -2808,7 +2814,7 @@
       <c r="A37" s="8">
         <v>6</v>
       </c>
-      <c r="B37" s="40"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="7" t="s">
         <v>15</v>
       </c>

</xml_diff>